<commit_message>
Con todos los excel funcionando
</commit_message>
<xml_diff>
--- a/app/Template/Reporte8.xlsx
+++ b/app/Template/Reporte8.xlsx
@@ -3,15 +3,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1790700" cy="533400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="User Image"/>
+        <xdr:cNvPr id="4" name="Imagen 3" descr="User Image"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -24,7 +24,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4857750" y="190500"/>
+          <a:off x="762000" y="459441"/>
           <a:ext cx="1790700" cy="533400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">

</xml_diff>

<commit_message>
Reportes con formato 12 y salidas con formato decimal
</commit_message>
<xml_diff>
--- a/app/Template/Reporte8.xlsx
+++ b/app/Template/Reporte8.xlsx
@@ -3,15 +3,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1790700" cy="533400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3" descr="User Image"/>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="User Image"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -24,7 +24,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="762000" y="459441"/>
+          <a:off x="4857750" y="190500"/>
           <a:ext cx="1790700" cy="533400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">

</xml_diff>